<commit_message>
Added `sortedHorizBarChart.` TO DO: fix not-rendered 'All Member States'
</commit_message>
<xml_diff>
--- a/JAF2R_shinylive -- logic.xlsx
+++ b/JAF2R_shinylive -- logic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eceuropaeu-my.sharepoint.com/personal/aleksander_rutkowski_ec_europa_eu/Documents/JAF2R_shinylive/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="160" documentId="8_{D0F80D74-D2A2-4954-97CB-5426C564C797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FAEB7736-0850-417F-AF5E-95217B82294F}"/>
+  <xr:revisionPtr revIDLastSave="192" documentId="8_{D0F80D74-D2A2-4954-97CB-5426C564C797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90B69AEE-1F38-4BAC-B276-BCF25EBDBD96}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="18796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -81,15 +81,6 @@
     <t>PlotType</t>
   </si>
   <si>
-    <t>grey histogram of all countries with the selected geo, 0, p25, p75, min, max as lines</t>
-  </si>
-  <si>
-    <t>grey histogram of all countries with the selected geo and eu, p25, p75, min, max as lines</t>
-  </si>
-  <si>
-    <t>bar chart similar to old PNG</t>
-  </si>
-  <si>
     <t>sorted bar chart</t>
   </si>
   <si>
@@ -139,6 +130,15 @@
   </si>
   <si>
     <t>y</t>
+  </si>
+  <si>
+    <t>grey histogram of all countries with the selected geo and median, eu, p25, p75,as lines</t>
+  </si>
+  <si>
+    <t>series of plots broadly similar to old PNG (but now with ore info)</t>
+  </si>
+  <si>
+    <t>sortedHorizBarChart</t>
   </si>
 </sst>
 </file>
@@ -233,7 +233,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -271,6 +271,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -576,11 +577,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="N2" sqref="N2:N17"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -591,7 +592,7 @@
     <col min="4" max="4" width="13.06640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="39.86328125" customWidth="1"/>
     <col min="6" max="6" width="25.3984375" customWidth="1"/>
-    <col min="7" max="7" width="14.9296875" customWidth="1"/>
+    <col min="7" max="7" width="16.59765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1" ht="34.9" customHeight="1" x14ac:dyDescent="0.45">
@@ -611,22 +612,22 @@
         <v>6</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I1" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="10" t="s">
         <v>23</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="K1" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="L1" s="10" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.45">
@@ -643,11 +644,11 @@
         <v>4</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I2" s="11" t="str">
         <f>IF(A2="multiple","i&gt;1","i==1")</f>
@@ -684,31 +685,31 @@
         <v>4</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="5" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="I3" s="11" t="str">
-        <f t="shared" ref="I3:I17" si="0">IF(A3="multiple","i&gt;1","i==1")</f>
-        <v>i&gt;1</v>
+        <f>IF(A3="multiple","i&gt; 1","i==1")</f>
+        <v>i&gt; 1</v>
       </c>
       <c r="J3" s="11" t="str">
-        <f t="shared" ref="J3:J17" si="1">IF(B3,"s","!s")</f>
-        <v>s</v>
+        <f>IF(B3," s","!s")</f>
+        <v xml:space="preserve"> s</v>
       </c>
       <c r="K3" s="11" t="str">
-        <f t="shared" ref="K3:K17" si="2">IF(C3="multiple","g&gt;1","g==1")</f>
+        <f>IF(C3="multiple","g&gt; 1","g==1")</f>
         <v>g==1</v>
       </c>
       <c r="L3" s="11" t="str">
-        <f t="shared" ref="L3:L17" si="3">IF(D3="multiple","y","!y")</f>
+        <f>IF(D3="multiple"," y","!y")</f>
         <v>!y</v>
       </c>
       <c r="N3" s="12" t="str">
-        <f t="shared" ref="N3:N17" si="4">"if("&amp;_xlfn.TEXTJOIN(" &amp;&amp; ",FALSE,I3:L3)&amp;") return("&amp;G3&amp;".(input))"&amp;" # "&amp;F3</f>
-        <v xml:space="preserve">if(i&gt;1 &amp;&amp; s &amp;&amp; g==1 &amp;&amp; !y) return(sortedBarChart.(input)) # </v>
+        <f t="shared" ref="N3:N17" si="0">"if("&amp;_xlfn.TEXTJOIN(" &amp;&amp; ",FALSE,I3:L3)&amp;") return("&amp;G3&amp;".(input))"&amp;" # "&amp;F3</f>
+        <v xml:space="preserve">if(i&gt; 1 &amp;&amp;  s &amp;&amp; g==1 &amp;&amp; !y) return(sortedHorizBarChart.(input)) # </v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.45">
@@ -725,31 +726,31 @@
         <v>4</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I4" s="11" t="str">
+        <f t="shared" ref="I4:I17" si="1">IF(A4="multiple","i&gt; 1","i==1")</f>
+        <v>i==1</v>
+      </c>
+      <c r="J4" s="11" t="str">
+        <f t="shared" ref="J4:J17" si="2">IF(B4," s","!s")</f>
+        <v xml:space="preserve"> s</v>
+      </c>
+      <c r="K4" s="11" t="str">
+        <f t="shared" ref="K4:K17" si="3">IF(C4="multiple","g&gt; 1","g==1")</f>
+        <v>g&gt; 1</v>
+      </c>
+      <c r="L4" s="11" t="str">
+        <f t="shared" ref="L4:L17" si="4">IF(D4="multiple"," y","!y")</f>
+        <v>!y</v>
+      </c>
+      <c r="N4" s="12" t="str">
         <f t="shared" si="0"/>
-        <v>i==1</v>
-      </c>
-      <c r="J4" s="11" t="str">
-        <f t="shared" si="1"/>
-        <v>s</v>
-      </c>
-      <c r="K4" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>g&gt;1</v>
-      </c>
-      <c r="L4" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>!y</v>
-      </c>
-      <c r="N4" s="12" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">if(i==1 &amp;&amp; s &amp;&amp; g&gt;1 &amp;&amp; !y) return(sortedBarChart.(input)) # </v>
+        <v xml:space="preserve">if(i==1 &amp;&amp;  s &amp;&amp; g&gt; 1 &amp;&amp; !y) return(sortedBarChart.(input)) # </v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.45">
@@ -766,31 +767,31 @@
         <v>4</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I5" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>i&gt; 1</v>
+      </c>
+      <c r="J5" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> s</v>
+      </c>
+      <c r="K5" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>g&gt; 1</v>
+      </c>
+      <c r="L5" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>!y</v>
+      </c>
+      <c r="N5" s="12" t="str">
         <f t="shared" si="0"/>
-        <v>i&gt;1</v>
-      </c>
-      <c r="J5" s="11" t="str">
-        <f t="shared" si="1"/>
-        <v>s</v>
-      </c>
-      <c r="K5" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>g&gt;1</v>
-      </c>
-      <c r="L5" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>!y</v>
-      </c>
-      <c r="N5" s="12" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">if(i&gt;1 &amp;&amp; s &amp;&amp; g&gt;1 &amp;&amp; !y) return(heatmapGrid.(input)) # </v>
+        <v xml:space="preserve">if(i&gt; 1 &amp;&amp;  s &amp;&amp; g&gt; 1 &amp;&amp; !y) return(heatmapGrid.(input)) # </v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.45">
@@ -808,34 +809,34 @@
       </c>
       <c r="E6" s="5" t="str">
         <f>E2</f>
-        <v>grey histogram of all countries with the selected geo, 0, p25, p75, min, max as lines</v>
+        <v>grey histogram of all countries with the selected geo and median, eu, p25, p75,as lines</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G6" s="5" t="str">
         <f>G2</f>
         <v>hist</v>
       </c>
       <c r="I6" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>i==1</v>
+      </c>
+      <c r="J6" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> s</v>
+      </c>
+      <c r="K6" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>g==1</v>
+      </c>
+      <c r="L6" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> y</v>
+      </c>
+      <c r="N6" s="12" t="str">
         <f t="shared" si="0"/>
-        <v>i==1</v>
-      </c>
-      <c r="J6" s="11" t="str">
-        <f t="shared" si="1"/>
-        <v>s</v>
-      </c>
-      <c r="K6" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>g==1</v>
-      </c>
-      <c r="L6" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>y</v>
-      </c>
-      <c r="N6" s="12" t="str">
-        <f t="shared" si="4"/>
-        <v>if(i==1 &amp;&amp; s &amp;&amp; g==1 &amp;&amp; y) return(hist.(input)) # multiple years ignored -- showing only the latest year</v>
+        <v>if(i==1 &amp;&amp;  s &amp;&amp; g==1 &amp;&amp;  y) return(hist.(input)) # multiple years ignored -- showing only the latest year</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.45">
@@ -856,31 +857,31 @@
         <v>sorted bar chart</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G7" s="5" t="str">
         <f t="shared" ref="G7:G9" si="6">G3</f>
-        <v>sortedBarChart</v>
+        <v>sortedHorizBarChart</v>
       </c>
       <c r="I7" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>i&gt; 1</v>
+      </c>
+      <c r="J7" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> s</v>
+      </c>
+      <c r="K7" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>g==1</v>
+      </c>
+      <c r="L7" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> y</v>
+      </c>
+      <c r="N7" s="12" t="str">
         <f t="shared" si="0"/>
-        <v>i&gt;1</v>
-      </c>
-      <c r="J7" s="11" t="str">
-        <f t="shared" si="1"/>
-        <v>s</v>
-      </c>
-      <c r="K7" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>g==1</v>
-      </c>
-      <c r="L7" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>y</v>
-      </c>
-      <c r="N7" s="12" t="str">
-        <f t="shared" si="4"/>
-        <v>if(i&gt;1 &amp;&amp; s &amp;&amp; g==1 &amp;&amp; y) return(sortedBarChart.(input)) # multiple years ignored -- showing only the latest year</v>
+        <v>if(i&gt; 1 &amp;&amp;  s &amp;&amp; g==1 &amp;&amp;  y) return(sortedHorizBarChart.(input)) # multiple years ignored -- showing only the latest year</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.45">
@@ -901,31 +902,31 @@
         <v>sorted bar chart</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G8" s="5" t="str">
         <f t="shared" si="6"/>
         <v>sortedBarChart</v>
       </c>
       <c r="I8" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>i==1</v>
+      </c>
+      <c r="J8" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> s</v>
+      </c>
+      <c r="K8" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>g&gt; 1</v>
+      </c>
+      <c r="L8" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> y</v>
+      </c>
+      <c r="N8" s="12" t="str">
         <f t="shared" si="0"/>
-        <v>i==1</v>
-      </c>
-      <c r="J8" s="11" t="str">
-        <f t="shared" si="1"/>
-        <v>s</v>
-      </c>
-      <c r="K8" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>g&gt;1</v>
-      </c>
-      <c r="L8" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>y</v>
-      </c>
-      <c r="N8" s="12" t="str">
-        <f t="shared" si="4"/>
-        <v>if(i==1 &amp;&amp; s &amp;&amp; g&gt;1 &amp;&amp; y) return(sortedBarChart.(input)) # multiple years ignored -- showing only the latest year</v>
+        <v>if(i==1 &amp;&amp;  s &amp;&amp; g&gt; 1 &amp;&amp;  y) return(sortedBarChart.(input)) # multiple years ignored -- showing only the latest year</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.45">
@@ -946,31 +947,31 @@
         <v>heatmap grid</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G9" s="5" t="str">
         <f t="shared" si="6"/>
         <v>heatmapGrid</v>
       </c>
       <c r="I9" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>i&gt; 1</v>
+      </c>
+      <c r="J9" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> s</v>
+      </c>
+      <c r="K9" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>g&gt; 1</v>
+      </c>
+      <c r="L9" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> y</v>
+      </c>
+      <c r="N9" s="12" t="str">
         <f t="shared" si="0"/>
-        <v>i&gt;1</v>
-      </c>
-      <c r="J9" s="11" t="str">
-        <f t="shared" si="1"/>
-        <v>s</v>
-      </c>
-      <c r="K9" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>g&gt;1</v>
-      </c>
-      <c r="L9" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>y</v>
-      </c>
-      <c r="N9" s="12" t="str">
-        <f t="shared" si="4"/>
-        <v>if(i&gt;1 &amp;&amp; s &amp;&amp; g&gt;1 &amp;&amp; y) return(heatmapGrid.(input)) # multiple years ignored -- showing only the latest year</v>
+        <v>if(i&gt; 1 &amp;&amp;  s &amp;&amp; g&gt; 1 &amp;&amp;  y) return(heatmapGrid.(input)) # multiple years ignored -- showing only the latest year</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.45">
@@ -987,30 +988,30 @@
         <v>4</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I10" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>i==1</v>
+      </c>
+      <c r="J10" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>!s</v>
+      </c>
+      <c r="K10" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>g==1</v>
+      </c>
+      <c r="L10" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>!y</v>
+      </c>
+      <c r="N10" s="12" t="str">
         <f t="shared" si="0"/>
-        <v>i==1</v>
-      </c>
-      <c r="J10" s="11" t="str">
-        <f t="shared" si="1"/>
-        <v>!s</v>
-      </c>
-      <c r="K10" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>g==1</v>
-      </c>
-      <c r="L10" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>!y</v>
-      </c>
-      <c r="N10" s="12" t="str">
-        <f t="shared" si="4"/>
         <v xml:space="preserve">if(i==1 &amp;&amp; !s &amp;&amp; g==1 &amp;&amp; !y) return(hist.(input)) # </v>
       </c>
     </row>
@@ -1028,33 +1029,33 @@
         <v>4</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I11" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>i&gt; 1</v>
+      </c>
+      <c r="J11" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>!s</v>
+      </c>
+      <c r="K11" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>g==1</v>
+      </c>
+      <c r="L11" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>!y</v>
+      </c>
+      <c r="N11" s="12" t="str">
         <f t="shared" si="0"/>
-        <v>i&gt;1</v>
-      </c>
-      <c r="J11" s="11" t="str">
-        <f t="shared" si="1"/>
-        <v>!s</v>
-      </c>
-      <c r="K11" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>g==1</v>
-      </c>
-      <c r="L11" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>!y</v>
-      </c>
-      <c r="N11" s="12" t="str">
-        <f t="shared" si="4"/>
-        <v>if(i&gt;1 &amp;&amp; !s &amp;&amp; g==1 &amp;&amp; !y) return(hist.(input)) # lapply(by indicator) due to different units</v>
+        <v>if(i&gt; 1 &amp;&amp; !s &amp;&amp; g==1 &amp;&amp; !y) return(hist.(input)) # lapply(by indicator) due to different units</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.45">
@@ -1071,31 +1072,31 @@
         <v>4</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I12" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>i==1</v>
+      </c>
+      <c r="J12" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>!s</v>
+      </c>
+      <c r="K12" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>g&gt; 1</v>
+      </c>
+      <c r="L12" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>!y</v>
+      </c>
+      <c r="N12" s="12" t="str">
         <f t="shared" si="0"/>
-        <v>i==1</v>
-      </c>
-      <c r="J12" s="11" t="str">
-        <f t="shared" si="1"/>
-        <v>!s</v>
-      </c>
-      <c r="K12" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>g&gt;1</v>
-      </c>
-      <c r="L12" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>!y</v>
-      </c>
-      <c r="N12" s="12" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">if(i==1 &amp;&amp; !s &amp;&amp; g&gt;1 &amp;&amp; !y) return(sortedBarChart.(input)) # </v>
+        <v xml:space="preserve">if(i==1 &amp;&amp; !s &amp;&amp; g&gt; 1 &amp;&amp; !y) return(sortedBarChart.(input)) # </v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.45">
@@ -1112,33 +1113,33 @@
         <v>4</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I13" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>i&gt; 1</v>
+      </c>
+      <c r="J13" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>!s</v>
+      </c>
+      <c r="K13" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>g&gt; 1</v>
+      </c>
+      <c r="L13" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>!y</v>
+      </c>
+      <c r="N13" s="12" t="str">
         <f t="shared" si="0"/>
-        <v>i&gt;1</v>
-      </c>
-      <c r="J13" s="11" t="str">
-        <f t="shared" si="1"/>
-        <v>!s</v>
-      </c>
-      <c r="K13" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>g&gt;1</v>
-      </c>
-      <c r="L13" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>!y</v>
-      </c>
-      <c r="N13" s="12" t="str">
-        <f t="shared" si="4"/>
-        <v>if(i&gt;1 &amp;&amp; !s &amp;&amp; g&gt;1 &amp;&amp; !y) return(sortedBarChart.(input)) # lapply(by indicator) due to different units</v>
+        <v>if(i&gt; 1 &amp;&amp; !s &amp;&amp; g&gt; 1 &amp;&amp; !y) return(sortedBarChart.(input)) # lapply(by indicator) due to different units</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.45">
@@ -1155,31 +1156,31 @@
         <v>5</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="I14" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>i==1</v>
+      </c>
+      <c r="J14" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>!s</v>
+      </c>
+      <c r="K14" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>g==1</v>
+      </c>
+      <c r="L14" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> y</v>
+      </c>
+      <c r="N14" s="12" t="str">
         <f t="shared" si="0"/>
-        <v>i==1</v>
-      </c>
-      <c r="J14" s="11" t="str">
-        <f t="shared" si="1"/>
-        <v>!s</v>
-      </c>
-      <c r="K14" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>g==1</v>
-      </c>
-      <c r="L14" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>y</v>
-      </c>
-      <c r="N14" s="12" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">if(i==1 &amp;&amp; !s &amp;&amp; g==1 &amp;&amp; y) return(linePlotGeoEU.(input)) # </v>
+        <v xml:space="preserve">if(i==1 &amp;&amp; !s &amp;&amp; g==1 &amp;&amp;  y) return(linePlotGeoEU.(input)) # </v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.45">
@@ -1196,33 +1197,33 @@
         <v>5</v>
       </c>
       <c r="E15" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>18</v>
-      </c>
       <c r="I15" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>i&gt; 1</v>
+      </c>
+      <c r="J15" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>!s</v>
+      </c>
+      <c r="K15" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>g==1</v>
+      </c>
+      <c r="L15" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> y</v>
+      </c>
+      <c r="N15" s="12" t="str">
         <f t="shared" si="0"/>
-        <v>i&gt;1</v>
-      </c>
-      <c r="J15" s="11" t="str">
-        <f t="shared" si="1"/>
-        <v>!s</v>
-      </c>
-      <c r="K15" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>g==1</v>
-      </c>
-      <c r="L15" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>y</v>
-      </c>
-      <c r="N15" s="12" t="str">
-        <f t="shared" si="4"/>
-        <v>if(i&gt;1 &amp;&amp; !s &amp;&amp; g==1 &amp;&amp; y) return(basicLinePlot.(input)) # lapply(by indicator) due to different units</v>
+        <v>if(i&gt; 1 &amp;&amp; !s &amp;&amp; g==1 &amp;&amp;  y) return(basicLinePlot.(input)) # lapply(by indicator) due to different units</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.45">
@@ -1239,31 +1240,31 @@
         <v>5</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I16" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>i==1</v>
+      </c>
+      <c r="J16" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>!s</v>
+      </c>
+      <c r="K16" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>g&gt; 1</v>
+      </c>
+      <c r="L16" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> y</v>
+      </c>
+      <c r="N16" s="12" t="str">
         <f t="shared" si="0"/>
-        <v>i==1</v>
-      </c>
-      <c r="J16" s="11" t="str">
-        <f t="shared" si="1"/>
-        <v>!s</v>
-      </c>
-      <c r="K16" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>g&gt;1</v>
-      </c>
-      <c r="L16" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>y</v>
-      </c>
-      <c r="N16" s="12" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">if(i==1 &amp;&amp; !s &amp;&amp; g&gt;1 &amp;&amp; y) return(basicLinePlot.(input)) # </v>
+        <v xml:space="preserve">if(i==1 &amp;&amp; !s &amp;&amp; g&gt; 1 &amp;&amp;  y) return(basicLinePlot.(input)) # </v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.45">
@@ -1280,33 +1281,33 @@
         <v>5</v>
       </c>
       <c r="E17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F17" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>18</v>
-      </c>
       <c r="I17" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>i&gt; 1</v>
+      </c>
+      <c r="J17" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>!s</v>
+      </c>
+      <c r="K17" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>g&gt; 1</v>
+      </c>
+      <c r="L17" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> y</v>
+      </c>
+      <c r="N17" s="12" t="str">
         <f t="shared" si="0"/>
-        <v>i&gt;1</v>
-      </c>
-      <c r="J17" s="11" t="str">
-        <f t="shared" si="1"/>
-        <v>!s</v>
-      </c>
-      <c r="K17" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v>g&gt;1</v>
-      </c>
-      <c r="L17" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>y</v>
-      </c>
-      <c r="N17" s="12" t="str">
-        <f t="shared" si="4"/>
-        <v>if(i&gt;1 &amp;&amp; !s &amp;&amp; g&gt;1 &amp;&amp; y) return(basicLinePlot.(input)) # lapply(by indicator) due to different units</v>
+        <v>if(i&gt; 1 &amp;&amp; !s &amp;&amp; g&gt; 1 &amp;&amp;  y) return(basicLinePlot.(input)) # lapply(by indicator) due to different units</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.45">
@@ -1314,13 +1315,13 @@
         <v>6</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="28.5" x14ac:dyDescent="0.45">
       <c r="E20" s="9" t="str" cm="1">
         <f t="array" ref="E20:F26">_xlfn.UNIQUE(_xlfn.HSTACK(E2:E17,G2:G17))</f>
-        <v>grey histogram of all countries with the selected geo, 0, p25, p75, min, max as lines</v>
+        <v>grey histogram of all countries with the selected geo and median, eu, p25, p75,as lines</v>
       </c>
       <c r="F20" s="9" t="str">
         <v>hist</v>
@@ -1331,28 +1332,28 @@
         <v>sorted bar chart</v>
       </c>
       <c r="F21" s="9" t="str">
-        <v>sortedBarChart</v>
+        <v>sortedHorizBarChart</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.45">
       <c r="E22" s="9" t="str">
-        <v>heatmap grid</v>
+        <v>sorted bar chart</v>
       </c>
       <c r="F22" s="9" t="str">
-        <v>heatmapGrid</v>
+        <v>sortedBarChart</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="28.5" x14ac:dyDescent="0.45">
       <c r="E23" s="9" t="str">
-        <v>grey histogram of all countries with the selected geo and eu, p25, p75, min, max as lines</v>
+        <v>heatmap grid</v>
       </c>
       <c r="F23" s="9" t="str">
-        <v>hist</v>
+        <v>heatmapGrid</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.45">
       <c r="E24" s="9" t="str">
-        <v>bar chart similar to old PNG</v>
+        <v>series of plots broadly similar to old PNG (but now with ore info)</v>
       </c>
       <c r="F24" s="9" t="str">
         <v>hist</v>
@@ -1367,11 +1368,57 @@
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="E26" s="9" t="str">
+      <c r="E26" s="13" t="str">
         <v>line plot</v>
       </c>
-      <c r="F26" s="9" t="str">
+      <c r="F26" s="13" t="str">
         <v>basicLinePlot</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="F28" t="str" cm="1">
+        <f t="array" ref="F28:F32">_xlfn.UNIQUE(F20:F25)</f>
+        <v>hist</v>
+      </c>
+      <c r="G28">
+        <f>COUNTIF($G$2:$G$17,F28)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="F29" t="str">
+        <v>sortedHorizBarChart</v>
+      </c>
+      <c r="G29">
+        <f t="shared" ref="G29:G32" si="7">COUNTIF($G$2:$G$17,F29)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="F30" t="str">
+        <v>sortedBarChart</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="F31" t="str">
+        <v>heatmapGrid</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="F32" t="str">
+        <v>linePlotGeoEU</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="7"/>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1385,6 +1432,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_activity xmlns="abe4fcb0-26a9-4b4f-826e-3f76808092f6" xsi:nil="true"/>
@@ -1392,7 +1448,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004F8954455CC87A47ADC9993F8A21564F" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2398e0c5c0211aee265904207da0d528">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="88bf217f-49c9-4146-840d-3aa20c401dac" xmlns:ns4="abe4fcb0-26a9-4b4f-826e-3f76808092f6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b662ec73f46367e518e20fb924e67fc7" ns3:_="" ns4:_="">
     <xsd:import namespace="88bf217f-49c9-4146-840d-3aa20c401dac"/>
@@ -1619,16 +1675,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69EBD776-8E68-4902-984C-3CC82B9FD9C1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0526181D-1296-48F4-890E-BDC3FC5F5F23}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -1645,7 +1700,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0237EA70-BE60-415C-8EE5-98A6FA5159F0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1662,12 +1717,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69EBD776-8E68-4902-984C-3CC82B9FD9C1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added table explaining the plot selection logic
</commit_message>
<xml_diff>
--- a/JAF2R_shinylive -- logic.xlsx
+++ b/JAF2R_shinylive -- logic.xlsx
@@ -2,18 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eceuropaeu-my.sharepoint.com/personal/aleksander_rutkowski_ec_europa_eu/Documents/JAF2R_shinylive/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="200" documentId="8_{D0F80D74-D2A2-4954-97CB-5426C564C797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{71AF4D0D-8582-4D3E-8E8A-55CC74206541}"/>
+  <xr:revisionPtr revIDLastSave="264" documentId="8_{D0F80D74-D2A2-4954-97CB-5426C564C797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E132DD4-5B28-4825-BF8E-3267B045A0ED}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="18796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="plot type combinations" sheetId="1" r:id="rId1"/>
+    <sheet name="For users" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'plot type combinations'!$A$1:$G$17</definedName>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="41">
   <si>
     <t>SelectedIndics</t>
   </si>
@@ -139,6 +140,48 @@
   </si>
   <si>
     <t>sortedHorizBarChart</t>
+  </si>
+  <si>
+    <t>Selecteded Indicators</t>
+  </si>
+  <si>
+    <t>Selected Scores</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Selected Countries</t>
+  </si>
+  <si>
+    <t>Selected Years</t>
+  </si>
+  <si>
+    <t>Histogram with additional data points highighted</t>
+  </si>
+  <si>
+    <t>Sorted Bar Chart</t>
+  </si>
+  <si>
+    <t>Heatmap Grid</t>
+  </si>
+  <si>
+    <t>Multiple Charts (one chart per indictor, due to different scales)</t>
+  </si>
+  <si>
+    <t>Line Plot with the selected country and EU distinguished, other countries all grey</t>
+  </si>
+  <si>
+    <t>Line Plot</t>
+  </si>
+  <si>
+    <t>Plot Type</t>
+  </si>
+  <si>
+    <t>not applcable (latest year available)</t>
   </si>
 </sst>
 </file>
@@ -148,7 +191,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,8 +227,23 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -204,8 +262,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -228,12 +292,132 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -272,6 +456,66 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -279,6 +523,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF0000FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -577,25 +826,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="N17" sqref="N2:N17"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2:G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.06640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.86328125" customWidth="1"/>
-    <col min="6" max="6" width="25.3984375" customWidth="1"/>
-    <col min="7" max="7" width="16.59765625" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.85546875" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" ht="34.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" s="1" customFormat="1" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -630,7 +880,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -671,7 +921,7 @@
         <v xml:space="preserve">if(i==1 &amp;&amp; s &amp;&amp; g==1 &amp;&amp; !y) return(hist.(input)) # </v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -712,7 +962,7 @@
         <v xml:space="preserve">if(i&gt; 1 &amp;&amp;  s &amp;&amp; g==1 &amp;&amp; !y) return(sortedHorizBarChart.(input)) # </v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -753,7 +1003,7 @@
         <v xml:space="preserve">if(i==1 &amp;&amp;  s &amp;&amp; g&gt; 1 &amp;&amp; !y) return(sortedBarChart.(input)) # </v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -794,7 +1044,7 @@
         <v xml:space="preserve">if(i&gt; 1 &amp;&amp;  s &amp;&amp; g&gt; 1 &amp;&amp; !y) return(heatmapGrid.(input)) # </v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -839,7 +1089,7 @@
         <v>if(i==1 &amp;&amp;  s &amp;&amp; g==1 &amp;&amp;  y) return(hist.(input)) # multiple years ignored -- showing only the latest year</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -884,7 +1134,7 @@
         <v>if(i&gt; 1 &amp;&amp;  s &amp;&amp; g==1 &amp;&amp;  y) return(sortedHorizBarChart.(input)) # multiple years ignored -- showing only the latest year</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
@@ -929,7 +1179,7 @@
         <v>if(i==1 &amp;&amp;  s &amp;&amp; g&gt; 1 &amp;&amp;  y) return(sortedBarChart.(input)) # multiple years ignored -- showing only the latest year</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
@@ -974,7 +1224,7 @@
         <v>if(i&gt; 1 &amp;&amp;  s &amp;&amp; g&gt; 1 &amp;&amp;  y) return(heatmapGrid.(input)) # multiple years ignored -- showing only the latest year</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>4</v>
       </c>
@@ -1015,7 +1265,7 @@
         <v xml:space="preserve">if(i==1 &amp;&amp; !s &amp;&amp; g==1 &amp;&amp; !y) return(hist.(input)) # </v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>5</v>
       </c>
@@ -1058,7 +1308,7 @@
         <v>if(i&gt; 1 &amp;&amp; !s &amp;&amp; g==1 &amp;&amp; !y) return(hist.(input)) # lapply(by indicator) due to different units</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>4</v>
       </c>
@@ -1099,7 +1349,7 @@
         <v xml:space="preserve">if(i==1 &amp;&amp; !s &amp;&amp; g&gt; 1 &amp;&amp; !y) return(sortedBarChart.(input)) # </v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>5</v>
       </c>
@@ -1142,7 +1392,7 @@
         <v>if(i&gt; 1 &amp;&amp; !s &amp;&amp; g&gt; 1 &amp;&amp; !y) return(sortedBarChart.(input)) # lapply(by indicator) due to different units</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>4</v>
       </c>
@@ -1185,7 +1435,7 @@
         <v>if(i==1 &amp;&amp; !s &amp;&amp; g==1 &amp;&amp;  y) return(linePlotGeoEU.(input)) # lapply(by indicator) due to different units</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>5</v>
       </c>
@@ -1228,7 +1478,7 @@
         <v>if(i&gt; 1 &amp;&amp; !s &amp;&amp; g==1 &amp;&amp;  y) return(linePlotGeoEU.(input)) # lapply(by indicator) due to different units</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>4</v>
       </c>
@@ -1269,7 +1519,7 @@
         <v xml:space="preserve">if(i==1 &amp;&amp; !s &amp;&amp; g&gt; 1 &amp;&amp;  y) return(basicLinePlot.(input)) # </v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>5</v>
       </c>
@@ -1312,7 +1562,7 @@
         <v>if(i&gt; 1 &amp;&amp; !s &amp;&amp; g&gt; 1 &amp;&amp;  y) return(basicLinePlot.(input)) # lapply(by indicator) due to different units</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E19" s="8" t="s">
         <v>6</v>
       </c>
@@ -1320,7 +1570,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="E20" s="9" t="str" cm="1">
         <f t="array" ref="E20:F26">_xlfn.UNIQUE(_xlfn.HSTACK(E2:E17,G2:G17))</f>
         <v>grey histogram of all countries with the selected geo and median, eu, p25, p75,as lines</v>
@@ -1329,7 +1579,7 @@
         <v>hist</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E21" s="9" t="str">
         <v>sorted bar chart</v>
       </c>
@@ -1337,7 +1587,7 @@
         <v>sortedHorizBarChart</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E22" s="9" t="str">
         <v>sorted bar chart</v>
       </c>
@@ -1345,7 +1595,7 @@
         <v>sortedBarChart</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E23" s="9" t="str">
         <v>heatmap grid</v>
       </c>
@@ -1353,7 +1603,7 @@
         <v>heatmapGrid</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="E24" s="9" t="str">
         <v>series of plots broadly similar to old PNG (but now with ore info)</v>
       </c>
@@ -1361,7 +1611,7 @@
         <v>hist</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="E25" s="9" t="str">
         <v>line plot with main lines = selected geo and EU, with other countries all light grey</v>
       </c>
@@ -1369,7 +1619,7 @@
         <v>linePlotGeoEU</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E26" s="13" t="str">
         <v>line plot</v>
       </c>
@@ -1377,7 +1627,7 @@
         <v>basicLinePlot</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F28" t="str" cm="1">
         <f t="array" ref="F28:F33">_xlfn.UNIQUE(F20:F26)</f>
         <v>hist</v>
@@ -1387,7 +1637,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F29" t="str">
         <v>sortedHorizBarChart</v>
       </c>
@@ -1396,7 +1646,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F30" t="str">
         <v>sortedBarChart</v>
       </c>
@@ -1405,7 +1655,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F31" t="str">
         <v>heatmapGrid</v>
       </c>
@@ -1414,7 +1664,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F32" t="str">
         <v>linePlotGeoEU</v>
       </c>
@@ -1423,7 +1673,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="6:7" x14ac:dyDescent="0.45">
+    <row r="33" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F33" t="str">
         <v>basicLinePlot</v>
       </c>
@@ -1442,7 +1692,309 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F8D87BC-9B58-4F66-9FD5-BE278B88973E}">
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F13" sqref="A1:F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.85546875" customWidth="1"/>
+    <col min="6" max="6" width="27.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="32" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="abe4fcb0-26a9-4b4f-826e-3f76808092f6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004F8954455CC87A47ADC9993F8A21564F" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2398e0c5c0211aee265904207da0d528">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="88bf217f-49c9-4146-840d-3aa20c401dac" xmlns:ns4="abe4fcb0-26a9-4b4f-826e-3f76808092f6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b662ec73f46367e518e20fb924e67fc7" ns3:_="" ns4:_="">
     <xsd:import namespace="88bf217f-49c9-4146-840d-3aa20c401dac"/>
@@ -1669,38 +2221,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="abe4fcb0-26a9-4b4f-826e-3f76808092f6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0237EA70-BE60-415C-8EE5-98A6FA5159F0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69EBD776-8E68-4902-984C-3CC82B9FD9C1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="88bf217f-49c9-4146-840d-3aa20c401dac"/>
-    <ds:schemaRef ds:uri="abe4fcb0-26a9-4b4f-826e-3f76808092f6"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1723,9 +2247,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69EBD776-8E68-4902-984C-3CC82B9FD9C1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0237EA70-BE60-415C-8EE5-98A6FA5159F0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="88bf217f-49c9-4146-840d-3aa20c401dac"/>
+    <ds:schemaRef ds:uri="abe4fcb0-26a9-4b4f-826e-3f76808092f6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>